<commit_message>
Update the Website List
</commit_message>
<xml_diff>
--- a/ScanningWebsiteAvailabilityTool/Data/WebsiteList.xlsx
+++ b/ScanningWebsiteAvailabilityTool/Data/WebsiteList.xlsx
@@ -24,15 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Website</t>
   </si>
   <si>
     <t>https://www.loseit.com/</t>
-  </si>
-  <si>
-    <t>http://ii-vfradev/Hackathon/</t>
   </si>
 </sst>
 </file>
@@ -350,7 +347,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -371,11 +368,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>